<commit_message>
#78-docs: Update ASVS checklist
</commit_message>
<xml_diff>
--- a/Deliverables/fase2-sprint2/content/ASVS_checklist.xlsx
+++ b/Deliverables/fase2-sprint2/content/ASVS_checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Veiga\RiderProjects\desofs2025_wed_pbs_1\Deliverables\fase2-sprint2\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B942CC5-1B4F-46C3-A339-B5967157D5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E70EE8-DFC5-4165-8B4E-E17C230DB69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -3526,7 +3526,7 @@
                   <c:v>91.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.411764705882355</c:v>
+                  <c:v>47.058823529411761</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>100</c:v>
@@ -3547,7 +3547,7 @@
                   <c:v>81.818181818181827</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>76.890756302521012</c:v>
+                  <c:v>78.151260504201687</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3878,7 +3878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -4042,7 +4042,7 @@
       </c>
       <c r="B9" s="9">
         <f>COUNTIF('Data Protection'!G2:G18,"Valid")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C9" s="10">
         <f>COUNTIF('Data Protection'!G2:G18,"&lt;&gt;Not Applicable")</f>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>29.411764705882355</v>
+        <v>47.058823529411761</v>
       </c>
       <c r="E9" s="12"/>
     </row>
@@ -4168,7 +4168,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4176,7 +4176,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>76.890756302521012</v>
+        <v>78.151260504201687</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -5826,7 +5826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -7476,17 +7476,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8943,16 +8943,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="A45:A51"/>
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -11394,8 +11394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
@@ -11729,7 +11729,7 @@
         <v>498</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
@@ -11751,7 +11751,7 @@
         <v>500</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
@@ -11795,7 +11795,7 @@
         <v>504</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>

</xml_diff>